<commit_message>
added accessType for queues
</commit_message>
<xml_diff>
--- a/input/samples/sample.xlsx
+++ b/input/samples/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgunadi/tools/ansible/solace_playbook/input/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49CC649-F0C3-4A4F-90E1-CDDF407EB2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F02FFA9-6391-494C-98E4-A93590A1E85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{C3A9B8EA-75FF-5248-AB06-BDBFE736BF1A}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{C3A9B8EA-75FF-5248-AB06-BDBFE736BF1A}"/>
   </bookViews>
   <sheets>
     <sheet name="msg-vpn" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="jndi_topic" localSheetId="9">'jndi-topic'!$A$1:$D$3</definedName>
     <definedName name="msg_vpn" localSheetId="0">'msg-vpn'!#REF!</definedName>
     <definedName name="msg_vpn_1" localSheetId="0">'msg-vpn'!$A$1:$O$2</definedName>
-    <definedName name="queue" localSheetId="5">queue!$A$1:$I$4</definedName>
+    <definedName name="queue" localSheetId="5">queue!$A$1:$J$4</definedName>
     <definedName name="queue_range" localSheetId="6">'queue-range'!$A$1:$M$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="113">
   <si>
     <t>msg_vpn</t>
   </si>
@@ -581,6 +581,15 @@
   </si>
   <si>
     <t>no-access</t>
+  </si>
+  <si>
+    <t>accessType</t>
+  </si>
+  <si>
+    <t>exclusive</t>
+  </si>
+  <si>
+    <t>non-exclusive</t>
   </si>
 </sst>
 </file>
@@ -987,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C16E4A-2948-2C42-8F9B-D762B87B00BD}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1636,26 +1645,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC61B8D-FDA0-5F41-BE4C-44476FDBBEAB}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1663,105 +1673,117 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>111</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>10000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>64</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="b">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>112</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>63</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>5000</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>65</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>112</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>109</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1000</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1918,7 +1940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535A1ABE-255A-4E46-B725-79D3ADC60E30}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>